<commit_message>
adding clk in crs
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesue\Documents\Cinvestav\Digital_proyects\uC_8bits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156EC7B2-A306-46AC-AE6C-E82792085993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BB8ED9-9E5A-4A97-A339-57060CAC6EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="-4980" windowWidth="18315" windowHeight="15585" xr2:uid="{712451C3-05C0-469D-8543-10018A5AC1B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{712451C3-05C0-469D-8543-10018A5AC1B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,19 +218,19 @@
     <t>Compares reg_a and reg_b; updates equality flag but stores no result.</t>
   </si>
   <si>
-    <t>RSHT</t>
-  </si>
-  <si>
     <t>0xE</t>
   </si>
   <si>
     <t>Right shifts reg_a by reg_b bits; result stored in reg_dst.</t>
   </si>
   <si>
-    <t>LSHT</t>
-  </si>
-  <si>
     <t>Left shifts reg_a by reg_b bits; result stored in reg_dst.</t>
+  </si>
+  <si>
+    <t>SHR</t>
+  </si>
+  <si>
+    <t>SHL</t>
   </si>
 </sst>
 </file>
@@ -397,21 +397,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,17 +421,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,7 +785,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -799,40 +799,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -841,120 +841,120 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15" t="s">
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -963,18 +963,18 @@
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -983,18 +983,18 @@
       <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1003,18 +1003,18 @@
       <c r="D12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1023,18 +1023,18 @@
       <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1043,18 +1043,18 @@
       <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1063,18 +1063,18 @@
       <c r="D15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1083,19 +1083,19 @@
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>16</v>
@@ -1103,31 +1103,31 @@
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1154,6 +1154,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="D9:E9"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="B1:E1"/>
@@ -1161,8 +1163,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>